<commit_message>
Actualización de archivos JSON y scripts 05 de noviembre
</commit_message>
<xml_diff>
--- a/Colmena.xlsx
+++ b/Colmena.xlsx
@@ -167,7 +167,11 @@
   </si>
   <si>
     <t>28/10/2025: Se han realizado las primeras extracciones con muy poco entrenamiento y ajustando regex como filtro inicial.
-31/10/2025: Se continúa trabajando en la extracción automatizada de información de documentos. Se prevé la entrega parcial de resultados durante la jornada, con la funcionalidad lista para validar en ambiente local.</t>
+31/10/2025: Se continúa trabajando en la extracción automatizada de información de documentos. Se prevé la entrega parcial de resultados durante la jornada, con la funcionalidad lista para validar en ambiente local.
+05/11/2025: El modelo ya identifica correctamente cuándo un documento corresponde a una incapacidad y cuándo no.
+Además, devuelve la información clave de la incapacidad, incluyendo el número de la hoja en la que se encuentra dentro del documento.
+Se implementó también el nuevo campo “Prórroga”, el cual está siendo extraído correctamente por el modelo durante el proceso de análisis.
+Actualmente, se planea realizar la implementación en el ambiente de test para validar el comportamiento integral del desarrollo.</t>
   </si>
   <si>
     <t>Jhon Bermudez</t>
@@ -190,8 +194,13 @@
 4.Resultado del proceso: Registrar y/o devolver los datos obtenidos para su uso en procesos posteriores de validación o integración.</t>
   </si>
   <si>
+    <t>FINALIZADO</t>
+  </si>
+  <si>
     <t>28/10/2025 Se valida método de consulta de manera manual y se descubre que a partir del consumo de una URL se puede hacer la consulta completa con los resultados que la plataforma retorna de manera visual
-29/10/2025 Se ajusta script para filtrar y trasformar la información de tal manera que sea útil para utilizarla</t>
+29/10/2025 Se ajusta script para filtrar y trasformar la información de tal manera que sea útil para utilizarla
+30/10/2025 Ajuste del scritp para mejorar el la respuesta
+31/10/2025 Se ejecutan la lista de NIT´s pendientes</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -222,9 +231,6 @@
   </si>
   <si>
     <t>Implementación de cartas (Devolución, glosa y pago).</t>
-  </si>
-  <si>
-    <t>FINALIZADO</t>
   </si>
   <si>
     <t>*02/10/2024 ya se encuentra implementado</t>
@@ -587,10 +593,10 @@
     <t>Internal Server Error</t>
   </si>
   <si>
-    <t>True</t>
+    <t>False</t>
   </si>
   <si>
-    <t>False</t>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -699,15 +705,15 @@
       <name val="Quattrocento Sans"/>
     </font>
     <font>
-      <b/>
       <u/>
-      <sz val="9"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Quattrocento Sans"/>
     </font>
     <font>
+      <b/>
       <u/>
-      <sz val="10"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Quattrocento Sans"/>
     </font>
@@ -1383,10 +1389,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2118,7 +2124,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2265,7 +2271,7 @@
         <v>22</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
@@ -2323,13 +2329,13 @@
       <c r="L3" s="23"/>
       <c r="M3" s="25">
         <f ca="1">IF(ISBLANK(L3), NETWORKDAYS(J3, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J3, L3, Hoja2!$A$1:$A$18))</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="29"/>
       <c r="P3" s="30"/>
       <c r="Q3" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
@@ -2385,13 +2391,13 @@
       <c r="L4" s="23"/>
       <c r="M4" s="25">
         <f ca="1">IF(ISBLANK(L4), NETWORKDAYS(J4, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J4, L4, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N4" s="23"/>
       <c r="O4" s="29"/>
       <c r="P4" s="34"/>
       <c r="Q4" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
@@ -2447,13 +2453,13 @@
       <c r="L5" s="23"/>
       <c r="M5" s="25">
         <f ca="1">IF(ISBLANK(L5), NETWORKDAYS(J5, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J5, L5, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N5" s="23"/>
       <c r="O5" s="29"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -2509,13 +2515,13 @@
       <c r="L6" s="36"/>
       <c r="M6" s="25">
         <f ca="1">IF(ISBLANK(L6), NETWORKDAYS(J6, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J6, L6, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
       <c r="P6" s="30"/>
       <c r="Q6" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
@@ -2557,13 +2563,13 @@
       <c r="L7" s="36"/>
       <c r="M7" s="25">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N7" s="42"/>
       <c r="O7" s="43"/>
       <c r="P7" s="34"/>
       <c r="Q7" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
@@ -2606,7 +2612,7 @@
         <v>26</v>
       </c>
       <c r="G8" s="19">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="22">
@@ -2619,7 +2625,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="25">
         <f ca="1">IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="43"/>
@@ -2627,7 +2633,7 @@
         <v>42</v>
       </c>
       <c r="Q8" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
@@ -2667,10 +2673,10 @@
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="18" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G9" s="19">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H9" s="20">
         <v>7</v>
@@ -2684,18 +2690,24 @@
       <c r="K9" s="24">
         <v>45966</v>
       </c>
-      <c r="L9" s="23"/>
+      <c r="L9" s="24">
+        <v>45961</v>
+      </c>
       <c r="M9" s="25">
         <f ca="1">IF(ISBLANK(L9), NETWORKDAYS(J9, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J9, L9, Hoja2!$A$1:$A$18))</f>
         <v>4</v>
       </c>
-      <c r="N9" s="23"/>
-      <c r="O9" s="43"/>
+      <c r="N9" s="24">
+        <v>45960</v>
+      </c>
+      <c r="O9" s="24">
+        <v>45960</v>
+      </c>
       <c r="P9" s="46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q9" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
@@ -2721,12 +2733,12 @@
       <c r="AM9" s="12"/>
     </row>
     <row r="10" spans="1:39" ht="53.25" customHeight="1">
-      <c r="A10" s="48"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="38"/>
       <c r="D10" s="39"/>
       <c r="E10" s="47"/>
-      <c r="F10" s="49"/>
+      <c r="F10" s="48"/>
       <c r="G10" s="40"/>
       <c r="H10" s="41"/>
       <c r="I10" s="33"/>
@@ -2735,7 +2747,7 @@
       <c r="L10" s="33"/>
       <c r="M10" s="25">
         <f ca="1">IF(ISBLANK(L10), NETWORKDAYS(J10, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J10, L10, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N10" s="42"/>
       <c r="O10" s="43"/>
@@ -2765,7 +2777,7 @@
       <c r="AM10" s="12"/>
     </row>
     <row r="11" spans="1:39" ht="53.25" customHeight="1">
-      <c r="A11" s="48"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="37"/>
       <c r="C11" s="38"/>
       <c r="D11" s="39"/>
@@ -2779,7 +2791,7 @@
       <c r="L11" s="23"/>
       <c r="M11" s="25">
         <f ca="1">IF(ISBLANK(L11), NETWORKDAYS(J11, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J11, L11, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N11" s="23"/>
       <c r="O11" s="43"/>
@@ -2809,7 +2821,7 @@
       <c r="AM11" s="12"/>
     </row>
     <row r="12" spans="1:39">
-      <c r="A12" s="48"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="37"/>
       <c r="C12" s="38"/>
       <c r="D12" s="39"/>
@@ -2823,7 +2835,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="25">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="43"/>
@@ -2853,7 +2865,7 @@
       <c r="AM12" s="12"/>
     </row>
     <row r="13" spans="1:39">
-      <c r="A13" s="48"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="37"/>
       <c r="C13" s="38"/>
       <c r="D13" s="39"/>
@@ -2867,7 +2879,7 @@
       <c r="L13" s="23"/>
       <c r="M13" s="25">
         <f ca="1">IF(ISBLANK(L13), NETWORKDAYS(J13, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J13, L13, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="43"/>
@@ -2897,7 +2909,7 @@
       <c r="AM13" s="12"/>
     </row>
     <row r="14" spans="1:39">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="37"/>
       <c r="C14" s="38"/>
       <c r="D14" s="39"/>
@@ -2911,7 +2923,7 @@
       <c r="L14" s="23"/>
       <c r="M14" s="25">
         <f ca="1">IF(ISBLANK(L14), NETWORKDAYS(J14, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J14, L14, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N14" s="23"/>
       <c r="O14" s="43"/>
@@ -2941,7 +2953,7 @@
       <c r="AM14" s="12"/>
     </row>
     <row r="15" spans="1:39">
-      <c r="A15" s="48"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="37"/>
       <c r="C15" s="38"/>
       <c r="D15" s="39"/>
@@ -2955,7 +2967,7 @@
       <c r="L15" s="23"/>
       <c r="M15" s="25">
         <f ca="1">IF(ISBLANK(L15), NETWORKDAYS(J15, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J15, L15, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N15" s="23"/>
       <c r="O15" s="43"/>
@@ -2985,7 +2997,7 @@
       <c r="AM15" s="12"/>
     </row>
     <row r="16" spans="1:39">
-      <c r="A16" s="48"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="37"/>
       <c r="C16" s="38"/>
       <c r="D16" s="39"/>
@@ -2999,7 +3011,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="25">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="43"/>
@@ -3029,7 +3041,7 @@
       <c r="AM16" s="12"/>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="48"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="37"/>
       <c r="C17" s="38"/>
       <c r="D17" s="39"/>
@@ -3043,7 +3055,7 @@
       <c r="L17" s="36"/>
       <c r="M17" s="25">
         <f ca="1">IF(ISBLANK(L17), NETWORKDAYS(J17, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J17, L17, Hoja2!$A$1:$A$18))</f>
-        <v>32814</v>
+        <v>32817</v>
       </c>
       <c r="N17" s="42"/>
       <c r="O17" s="43"/>
@@ -3073,7 +3085,7 @@
       <c r="AM17" s="12"/>
     </row>
     <row r="18" spans="1:39">
-      <c r="A18" s="48"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="37"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
@@ -3114,7 +3126,7 @@
       <c r="AM18" s="12"/>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="48"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="37"/>
       <c r="C19" s="38"/>
       <c r="D19" s="39"/>
@@ -3155,7 +3167,7 @@
       <c r="AM19" s="12"/>
     </row>
     <row r="20" spans="1:39">
-      <c r="A20" s="48"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="37"/>
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
@@ -40965,7 +40977,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="107" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" s="107" t="s">
         <v>2</v>
@@ -40992,13 +41004,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="110" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K1" s="107" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L1" s="111" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="112"/>
       <c r="N1" s="112"/>
@@ -41017,14 +41029,14 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="113" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="114" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="115"/>
       <c r="D2" s="116" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E2" s="117">
         <v>45526</v>
@@ -41038,7 +41050,7 @@
       <c r="J2" s="115"/>
       <c r="K2" s="115"/>
       <c r="L2" s="115" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M2" s="118"/>
       <c r="N2" s="118"/>
@@ -41057,16 +41069,16 @@
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" s="119" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="120" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" s="121" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D3" s="121" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E3" s="122">
         <v>45560</v>
@@ -41157,7 +41169,7 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="111" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="127" t="s">
         <v>65</v>
@@ -41255,10 +41267,10 @@
     </row>
     <row r="7" spans="1:26" ht="99.75">
       <c r="A7" s="111" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="120" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" s="139" t="s">
         <v>74</v>
@@ -41304,7 +41316,7 @@
     </row>
     <row r="8" spans="1:26" ht="71.25">
       <c r="A8" s="143" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="144" t="s">
         <v>76</v>
@@ -50000,7 +50012,7 @@
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="166" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="167" t="s">
         <v>115</v>
@@ -53284,7 +53296,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="173" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" s="173" t="s">
         <v>2</v>
@@ -53311,13 +53323,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="177" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K1" s="178" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L1" s="176" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="179"/>
       <c r="N1" s="179"/>
@@ -53343,7 +53355,7 @@
       </c>
       <c r="C2" s="182"/>
       <c r="D2" s="182" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E2" s="183">
         <v>45567</v>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 28  de noviembre
</commit_message>
<xml_diff>
--- a/Colmena.xlsx
+++ b/Colmena.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="EN PROCESO (Colmena)" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
     <t>Se solicita que al momento de capturar la informacion del formato de beneficiario final, el formulario que este marcado como NO tome los nuevos campos</t>
   </si>
   <si>
-    <t>PASO A PRODUCCION</t>
+    <t>FINALIZADO</t>
   </si>
   <si>
     <t>Se entrega el requerimiento de acuerdo con la solicitud del cliente</t>
@@ -112,9 +112,6 @@
 Reemplazar el campo de Sucursal por Regionales</t>
   </si>
   <si>
-    <t>EN PROCESO</t>
-  </si>
-  <si>
     <t>se entrega en produccion modificacion de informe de la manera solicitada</t>
   </si>
   <si>
@@ -127,7 +124,7 @@
     <t>Se requiere la creacion de un (chek) para cargue de afiliaciones contratos no vinculados que permita seleccionar varios contratos y de esta manera me genere los planos de los contratos seleccionaos en un solo LOG para garantizar un solo cargue que evite las demoras que actualmente se presentan al cargar estos contratos.</t>
   </si>
   <si>
-    <t>PENDIENTE</t>
+    <t>PRUEBAS ClIENTE</t>
   </si>
   <si>
     <t>SCTASK0339314</t>
@@ -138,6 +135,9 @@
   <si>
     <t>CAMPO TELEFONOS 
 Se requiere que en los casos donde los campos de teléfono para contratos dependientes y no vinculados  vengan vacíos y/o relacionen  información inconsistente como números repetidos o caracteres especiales se tome por defecto el numero de la empresa para evitar errores de cargue al momento de vincular contratos en APOLO.</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
   </si>
   <si>
     <t>SCTASK0340882</t>
@@ -169,12 +169,18 @@
 Este requerimiento busca automatizar la clasificación y extracción de datos relevantes, mejorando la precisión del proceso, reduciendo tiempos de validación y evitando errores humanos en la identificación de archivos.</t>
   </si>
   <si>
+    <t>EN PROCESO</t>
+  </si>
+  <si>
     <t>28/10/2025: Se han realizado las primeras extracciones con muy poco entrenamiento y ajustando regex como filtro inicial.
 31/10/2025: Se continúa trabajando en la extracción automatizada de información de documentos. Se prevé la entrega parcial de resultados durante la jornada, con la funcionalidad lista para validar en ambiente local.
 05/11/2025: El modelo ya identifica correctamente cuándo un documento corresponde a una incapacidad y cuándo no.
 Además, devuelve la información clave de la incapacidad, incluyendo el número de la hoja en la que se encuentra dentro del documento.
 Se implementó también el nuevo campo “Prórroga”, el cual está siendo extraído correctamente por el modelo durante el proceso de análisis.
-Actualmente, se planea realizar la implementación en el ambiente de test para validar el comportamiento integral del desarrollo.</t>
+Actualmente, se planea realizar la implementación en el ambiente de test para validar el comportamiento integral del desarrollo.
+24/11/2025: Se recibió información inicial y hubo primera reunión. Aún no se ha analizado la documentación recibida; avance estimado en 5%. Pendiente estructurar el análisis y organizar los insumos.
+Se presentó fallo por conflicto con una librería y cambios no deseados en la IP pública. Se desinstaló la VPN afectada. Hoy se destinará tiempo para intentar reinstalar paquetes o aprovechar el ambiente test existente.
+26/11/2025: Pendiente retomar los ajustes solicitados por Colmena. Se dedicará parte del día a trabajar con Jenry para avanzar, ya que no se pudo atender este requerimiento en días anteriores por priorización de otros temas.</t>
   </si>
   <si>
     <t>Jhon Bermudez</t>
@@ -195,9 +201,6 @@
 *Desde la sección “Información Básica” o “RUT”, obtener y almacenar el código CIIU correspondiente.
 *Desde la sección “Información Financiera”, recuperar el valor reportado en el campo “Ingresos Mensuales”.
 4.Resultado del proceso: Registrar y/o devolver los datos obtenidos para su uso en procesos posteriores de validación o integración.</t>
-  </si>
-  <si>
-    <t>FINALIZADO</t>
   </si>
   <si>
     <t>28/10/2025 Se valida método de consulta de manera manual y se descubre que a partir del consumo de una URL se puede hacer la consulta completa con los resultados que la plataforma retorna de manera visual
@@ -596,10 +599,10 @@
     <t>Internal Server Error</t>
   </si>
   <si>
-    <t>True</t>
+    <t>TRUE</t>
   </si>
   <si>
-    <t>False</t>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -2125,9 +2128,9 @@
   </sheetPr>
   <dimension ref="A1:AM940"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2314,10 +2317,10 @@
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G3" s="19">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H3" s="20">
         <v>30</v>
@@ -2332,12 +2335,12 @@
       <c r="L3" s="23"/>
       <c r="M3" s="25">
         <f ca="1">IF(ISBLANK(L3), NETWORKDAYS(J3, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J3, L3, Hoja2!$A$1:$A$18))</f>
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="29"/>
       <c r="P3" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="30" t="s">
         <v>149</v>
@@ -2370,17 +2373,17 @@
         <v>17</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="31" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>30</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="19">
         <v>0</v>
@@ -2396,7 +2399,7 @@
       <c r="L4" s="23"/>
       <c r="M4" s="25">
         <f ca="1">IF(ISBLANK(L4), NETWORKDAYS(J4, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J4, L4, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N4" s="23"/>
       <c r="O4" s="29"/>
@@ -2432,17 +2435,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="34" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>34</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G5" s="19">
         <v>0</v>
@@ -2458,7 +2461,7 @@
       <c r="L5" s="23"/>
       <c r="M5" s="25">
         <f ca="1">IF(ISBLANK(L5), NETWORKDAYS(J5, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J5, L5, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N5" s="23"/>
       <c r="O5" s="29"/>
@@ -2504,10 +2507,10 @@
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G6" s="19">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H6" s="20">
         <v>20</v>
@@ -2520,7 +2523,7 @@
       <c r="L6" s="36"/>
       <c r="M6" s="25">
         <f ca="1">IF(ISBLANK(L6), NETWORKDAYS(J6, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J6, L6, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
@@ -2568,7 +2571,7 @@
       <c r="L7" s="36"/>
       <c r="M7" s="25">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N7" s="42"/>
       <c r="O7" s="43"/>
@@ -2614,10 +2617,10 @@
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G8" s="19">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="22">
@@ -2630,12 +2633,12 @@
       <c r="L8" s="23"/>
       <c r="M8" s="25">
         <f ca="1">IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="43"/>
       <c r="P8" s="46" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q8" s="30" t="s">
         <v>149</v>
@@ -2665,20 +2668,20 @@
     </row>
     <row r="9" spans="1:39" ht="53.25" customHeight="1">
       <c r="A9" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="18" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G9" s="19">
         <v>100</v>
@@ -2752,7 +2755,7 @@
       <c r="L10" s="32"/>
       <c r="M10" s="25">
         <f ca="1">IF(ISBLANK(L10), NETWORKDAYS(J10, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J10, L10, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N10" s="42"/>
       <c r="O10" s="43"/>
@@ -2796,7 +2799,7 @@
       <c r="L11" s="23"/>
       <c r="M11" s="25">
         <f ca="1">IF(ISBLANK(L11), NETWORKDAYS(J11, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J11, L11, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N11" s="23"/>
       <c r="O11" s="43"/>
@@ -2840,7 +2843,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="25">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="43"/>
@@ -2884,7 +2887,7 @@
       <c r="L13" s="23"/>
       <c r="M13" s="25">
         <f ca="1">IF(ISBLANK(L13), NETWORKDAYS(J13, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J13, L13, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="43"/>
@@ -2928,7 +2931,7 @@
       <c r="L14" s="23"/>
       <c r="M14" s="25">
         <f ca="1">IF(ISBLANK(L14), NETWORKDAYS(J14, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J14, L14, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N14" s="23"/>
       <c r="O14" s="43"/>
@@ -2972,7 +2975,7 @@
       <c r="L15" s="23"/>
       <c r="M15" s="25">
         <f ca="1">IF(ISBLANK(L15), NETWORKDAYS(J15, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J15, L15, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N15" s="23"/>
       <c r="O15" s="43"/>
@@ -3016,7 +3019,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="25">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="43"/>
@@ -3060,7 +3063,7 @@
       <c r="L17" s="36"/>
       <c r="M17" s="25">
         <f ca="1">IF(ISBLANK(L17), NETWORKDAYS(J17, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J17, L17, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32834</v>
       </c>
       <c r="N17" s="42"/>
       <c r="O17" s="43"/>
@@ -40939,11 +40942,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F940">
+      <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS ClIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
+    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L940 N2:O940">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F940">
-      <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS NACOL,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -41083,7 +41086,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="121" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="E3" s="122">
         <v>45560</v>
@@ -53360,7 +53363,7 @@
       </c>
       <c r="C2" s="182"/>
       <c r="D2" s="182" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="E2" s="183">
         <v>45567</v>
@@ -53411,7 +53414,7 @@
         <v>143</v>
       </c>
       <c r="D3" s="182" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E3" s="183">
         <v>45575</v>
@@ -53456,7 +53459,7 @@
         <v>145</v>
       </c>
       <c r="D4" s="182" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E4" s="183">
         <v>45575</v>
@@ -53503,7 +53506,7 @@
         <v>148</v>
       </c>
       <c r="D5" s="182" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E5" s="183">
         <v>45575</v>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 21  de enero 2026
</commit_message>
<xml_diff>
--- a/Colmena.xlsx
+++ b/Colmena.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="188">
   <si>
     <t>Asignado a</t>
   </si>
@@ -250,11 +250,9 @@
     <t>Automatizacion de SAT independientes</t>
   </si>
   <si>
-    <t>PAUSADO</t>
-  </si>
-  <si>
     <t xml:space="preserve">20251218, se requiere permisos para conmexion a las urls de consumo del api, se valida con
- tecnologia de colmena, aun no dan el permiso solicitado, por lo tanto se mantiene en espera </t>
+ tecnologia de colmena, aun no dan el permiso solicitado, por lo tanto se mantiene en espera 
+20260116 ya se concedieron permisos para la conexion a la url de preubas de la consulta, se probo conexiones y funciona, se indica a colmena para identificar el apso a seguir </t>
   </si>
   <si>
     <t>MEJORA_4</t>
@@ -288,13 +286,13 @@
     <t xml:space="preserve">actualizacion cargue masivo listados </t>
   </si>
   <si>
-    <t>PRUEBAS IMAGINE</t>
-  </si>
-  <si>
     <t>MEJORA_8</t>
   </si>
   <si>
     <t>mejora informe estadisticos imagine</t>
+  </si>
+  <si>
+    <t>PRUEBAS IMAGINE</t>
   </si>
   <si>
     <t>MEJORA_9</t>
@@ -723,7 +721,7 @@
     <t>True</t>
   </si>
   <si>
-    <t>false</t>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -2269,7 +2267,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2416,7 +2414,7 @@
         <v>22</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
@@ -2474,7 +2472,7 @@
       <c r="L3" s="23"/>
       <c r="M3" s="25">
         <f ca="1">IF(ISBLANK(L3), NETWORKDAYS(J3, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J3, L3, Hoja2!$A$1:$A$18))</f>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="29"/>
@@ -2482,7 +2480,7 @@
         <v>26</v>
       </c>
       <c r="Q3" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
@@ -2546,7 +2544,7 @@
         <v>30</v>
       </c>
       <c r="Q4" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
@@ -2602,13 +2600,13 @@
       <c r="L5" s="23"/>
       <c r="M5" s="25">
         <f ca="1">IF(ISBLANK(L5), NETWORKDAYS(J5, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J5, L5, Hoja2!$A$1:$A$18))</f>
-        <v>32870</v>
+        <v>32872</v>
       </c>
       <c r="N5" s="23"/>
       <c r="O5" s="29"/>
       <c r="P5" s="35"/>
       <c r="Q5" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -2664,13 +2662,13 @@
       <c r="L6" s="36"/>
       <c r="M6" s="25">
         <f ca="1">IF(ISBLANK(L6), NETWORKDAYS(J6, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J6, L6, Hoja2!$A$1:$A$18))</f>
-        <v>32870</v>
+        <v>32872</v>
       </c>
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
       <c r="P6" s="35"/>
       <c r="Q6" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
@@ -2712,13 +2710,13 @@
       <c r="L7" s="36"/>
       <c r="M7" s="25">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32870</v>
+        <v>32872</v>
       </c>
       <c r="N7" s="42"/>
       <c r="O7" s="43"/>
       <c r="P7" s="44"/>
-      <c r="Q7" s="30" t="b">
-        <v>0</v>
+      <c r="Q7" s="30" t="s">
+        <v>187</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
@@ -2774,7 +2772,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="25">
         <f ca="1">IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="43"/>
@@ -2782,7 +2780,7 @@
         <v>44</v>
       </c>
       <c r="Q8" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
@@ -2856,7 +2854,7 @@
         <v>49</v>
       </c>
       <c r="Q9" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
@@ -2904,8 +2902,8 @@
       <c r="N10" s="42"/>
       <c r="O10" s="43"/>
       <c r="P10" s="44"/>
-      <c r="Q10" t="s">
-        <v>188</v>
+      <c r="Q10" s="27" t="s">
+        <v>187</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
@@ -2976,7 +2974,7 @@
         <v>55</v>
       </c>
       <c r="Q11" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
@@ -3047,7 +3045,7 @@
         <v>59</v>
       </c>
       <c r="Q12" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
@@ -3087,7 +3085,7 @@
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="54" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="G13" s="19">
         <v>15</v>
@@ -3101,10 +3099,10 @@
       <c r="N13" s="23"/>
       <c r="O13" s="43"/>
       <c r="P13" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q13" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
@@ -3134,13 +3132,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="D14" s="56" t="s">
         <v>65</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>66</v>
       </c>
       <c r="E14" s="57"/>
       <c r="F14" s="54" t="s">
@@ -3170,10 +3168,10 @@
         <v>46027</v>
       </c>
       <c r="P14" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q14" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
@@ -3203,10 +3201,10 @@
         <v>17</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="48" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>69</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="60"/>
@@ -3238,7 +3236,7 @@
       </c>
       <c r="P15" s="35"/>
       <c r="Q15" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
@@ -3268,10 +3266,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="48" t="s">
         <v>70</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>71</v>
       </c>
       <c r="D16" s="39"/>
       <c r="E16" s="17"/>
@@ -3303,7 +3301,7 @@
       </c>
       <c r="P16" s="35"/>
       <c r="Q16" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
@@ -3333,18 +3331,18 @@
         <v>17</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="48" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>73</v>
       </c>
       <c r="D17" s="39"/>
       <c r="E17" s="17"/>
       <c r="F17" s="54" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="G17" s="19">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="H17" s="41"/>
       <c r="I17" s="46">
@@ -3368,7 +3366,7 @@
       </c>
       <c r="P17" s="35"/>
       <c r="Q17" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
@@ -3398,15 +3396,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="17"/>
       <c r="F18" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G18" s="19">
         <v>95</v>
@@ -3433,7 +3431,7 @@
       </c>
       <c r="P18" s="35"/>
       <c r="Q18" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
@@ -3463,17 +3461,17 @@
         <v>17</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="D19" s="56" t="s">
         <v>78</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>79</v>
       </c>
       <c r="E19" s="63"/>
       <c r="F19" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G19" s="19">
         <v>80</v>
@@ -3494,7 +3492,7 @@
       <c r="O19" s="43"/>
       <c r="P19" s="35"/>
       <c r="Q19" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
@@ -3524,13 +3522,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="D20" s="56" t="s">
         <v>81</v>
-      </c>
-      <c r="D20" s="56" t="s">
-        <v>82</v>
       </c>
       <c r="E20" s="63"/>
       <c r="F20" s="51" t="s">
@@ -3554,10 +3552,10 @@
       <c r="N20" s="36"/>
       <c r="O20" s="36"/>
       <c r="P20" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q20" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
@@ -3587,10 +3585,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="48" t="s">
         <v>84</v>
-      </c>
-      <c r="C21" s="48" t="s">
-        <v>85</v>
       </c>
       <c r="D21" s="39"/>
       <c r="E21" s="63"/>
@@ -3616,7 +3614,7 @@
       <c r="O21" s="43"/>
       <c r="P21" s="35"/>
       <c r="Q21" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
@@ -3646,15 +3644,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="48" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>87</v>
       </c>
       <c r="D22" s="39"/>
       <c r="E22" s="63"/>
       <c r="F22" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="64">
         <v>80</v>
@@ -3681,7 +3679,7 @@
       </c>
       <c r="P22" s="35"/>
       <c r="Q22" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
@@ -41394,7 +41392,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="115" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="115" t="s">
         <v>2</v>
@@ -41421,13 +41419,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="118" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="115" t="s">
+      <c r="L1" s="119" t="s">
         <v>91</v>
-      </c>
-      <c r="L1" s="119" t="s">
-        <v>92</v>
       </c>
       <c r="M1" s="120"/>
       <c r="N1" s="120"/>
@@ -41446,14 +41444,14 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="121" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="122" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="122" t="s">
-        <v>94</v>
       </c>
       <c r="C2" s="123"/>
       <c r="D2" s="124" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="125">
         <v>45526</v>
@@ -41467,7 +41465,7 @@
       <c r="J2" s="123"/>
       <c r="K2" s="123"/>
       <c r="L2" s="123" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M2" s="126"/>
       <c r="N2" s="126"/>
@@ -41486,13 +41484,13 @@
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" s="127" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="128" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="129" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" s="129" t="s">
-        <v>98</v>
       </c>
       <c r="D3" s="129" t="s">
         <v>21</v>
@@ -41516,7 +41514,7 @@
       </c>
       <c r="K3" s="131"/>
       <c r="L3" s="133" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M3" s="120"/>
       <c r="N3" s="120"/>
@@ -41535,16 +41533,16 @@
     </row>
     <row r="4" spans="1:26" ht="186">
       <c r="A4" s="134" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="135" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="C4" s="134" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="134" t="s">
+      <c r="D4" s="136" t="s">
         <v>102</v>
-      </c>
-      <c r="D4" s="136" t="s">
-        <v>103</v>
       </c>
       <c r="E4" s="137">
         <v>45581</v>
@@ -41567,7 +41565,7 @@
       </c>
       <c r="K4" s="137"/>
       <c r="L4" s="134" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M4" s="140"/>
       <c r="N4" s="140"/>
@@ -41586,16 +41584,16 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="119" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="135" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="129" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="129" t="s">
-        <v>106</v>
-      </c>
       <c r="D5" s="141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="130">
         <v>45572</v>
@@ -41616,7 +41614,7 @@
       </c>
       <c r="K5" s="130"/>
       <c r="L5" s="133" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M5" s="120"/>
       <c r="N5" s="120"/>
@@ -41635,16 +41633,16 @@
     </row>
     <row r="6" spans="1:26" ht="117">
       <c r="A6" s="142" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="142" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="142" t="s">
+      <c r="C6" s="136" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="136" t="s">
+      <c r="D6" s="142" t="s">
         <v>110</v>
-      </c>
-      <c r="D6" s="142" t="s">
-        <v>111</v>
       </c>
       <c r="E6" s="143">
         <v>45602</v>
@@ -41665,7 +41663,7 @@
         <v>45602</v>
       </c>
       <c r="L6" s="144" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M6" s="145"/>
       <c r="N6" s="146"/>
@@ -41684,16 +41682,16 @@
     </row>
     <row r="7" spans="1:26" ht="99.75">
       <c r="A7" s="119" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="128" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="147" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" s="141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="130">
         <v>45589</v>
@@ -41714,7 +41712,7 @@
       </c>
       <c r="K7" s="141"/>
       <c r="L7" s="149" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M7" s="150"/>
       <c r="N7" s="150"/>
@@ -41733,14 +41731,14 @@
     </row>
     <row r="8" spans="1:26" ht="71.25">
       <c r="A8" s="151" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="152" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="153"/>
       <c r="D8" s="153" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="154">
         <v>45603</v>
@@ -41761,7 +41759,7 @@
       </c>
       <c r="K8" s="154"/>
       <c r="L8" s="156" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M8" s="120"/>
       <c r="N8" s="120"/>
@@ -41780,16 +41778,16 @@
     </row>
     <row r="9" spans="1:26" ht="42.75">
       <c r="A9" s="157" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="158" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="C9" s="159" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="159" t="s">
+      <c r="D9" s="160" t="s">
         <v>120</v>
-      </c>
-      <c r="D9" s="160" t="s">
-        <v>121</v>
       </c>
       <c r="E9" s="161">
         <v>45671</v>
@@ -41798,7 +41796,7 @@
         <v>45673</v>
       </c>
       <c r="G9" s="159" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H9" s="161">
         <v>45680</v>
@@ -41812,7 +41810,7 @@
       </c>
       <c r="K9" s="159"/>
       <c r="L9" s="163" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M9" s="164"/>
       <c r="N9" s="164"/>
@@ -41831,14 +41829,14 @@
     </row>
     <row r="10" spans="1:26" ht="57">
       <c r="A10" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="165"/>
       <c r="C10" s="163" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" s="161">
         <v>45671</v>
@@ -41857,7 +41855,7 @@
       <c r="J10" s="159"/>
       <c r="K10" s="159"/>
       <c r="L10" s="163" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M10" s="164"/>
       <c r="N10" s="164"/>
@@ -41876,14 +41874,14 @@
     </row>
     <row r="11" spans="1:26" ht="42.75">
       <c r="A11" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="165"/>
       <c r="C11" s="163" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D11" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="161">
         <v>45671</v>
@@ -41902,7 +41900,7 @@
       <c r="J11" s="159"/>
       <c r="K11" s="159"/>
       <c r="L11" s="163" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M11" s="164"/>
       <c r="N11" s="164"/>
@@ -41921,14 +41919,14 @@
     </row>
     <row r="12" spans="1:26" ht="42.75">
       <c r="A12" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="165"/>
       <c r="C12" s="163" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="161">
         <v>45671</v>
@@ -41947,7 +41945,7 @@
       <c r="J12" s="159"/>
       <c r="K12" s="159"/>
       <c r="L12" s="163" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M12" s="164"/>
       <c r="N12" s="164"/>
@@ -41966,14 +41964,14 @@
     </row>
     <row r="13" spans="1:26" ht="42.75">
       <c r="A13" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" s="165"/>
       <c r="C13" s="163" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E13" s="161">
         <v>45671</v>
@@ -41992,7 +41990,7 @@
       <c r="J13" s="159"/>
       <c r="K13" s="159"/>
       <c r="L13" s="163" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M13" s="164"/>
       <c r="N13" s="164"/>
@@ -42011,14 +42009,14 @@
     </row>
     <row r="14" spans="1:26" ht="42.75">
       <c r="A14" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" s="165"/>
       <c r="C14" s="163" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E14" s="161">
         <v>45671</v>
@@ -42037,7 +42035,7 @@
       <c r="J14" s="159"/>
       <c r="K14" s="159"/>
       <c r="L14" s="159" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M14" s="164"/>
       <c r="N14" s="164"/>
@@ -42056,14 +42054,14 @@
     </row>
     <row r="15" spans="1:26" ht="42.75">
       <c r="A15" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" s="165"/>
       <c r="C15" s="163" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E15" s="161">
         <v>45671</v>
@@ -42082,7 +42080,7 @@
       <c r="J15" s="159"/>
       <c r="K15" s="159"/>
       <c r="L15" s="159" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M15" s="164"/>
       <c r="N15" s="164"/>
@@ -42101,14 +42099,14 @@
     </row>
     <row r="16" spans="1:26" ht="71.25">
       <c r="A16" s="157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" s="166"/>
       <c r="C16" s="167" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D16" s="160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E16" s="161">
         <v>45681</v>
@@ -42127,7 +42125,7 @@
       <c r="J16" s="159"/>
       <c r="K16" s="159"/>
       <c r="L16" s="163" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M16" s="164"/>
       <c r="N16" s="164"/>
@@ -48659,7 +48657,7 @@
         <v>45292</v>
       </c>
       <c r="B1" s="164" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
@@ -48667,7 +48665,7 @@
         <v>45299</v>
       </c>
       <c r="B2" s="164" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -48675,7 +48673,7 @@
         <v>45376</v>
       </c>
       <c r="B3" s="164" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
@@ -48683,7 +48681,7 @@
         <v>45379</v>
       </c>
       <c r="B4" s="164" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -48691,7 +48689,7 @@
         <v>45380</v>
       </c>
       <c r="B5" s="164" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
@@ -48699,7 +48697,7 @@
         <v>45413</v>
       </c>
       <c r="B6" s="164" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -48707,7 +48705,7 @@
         <v>45425</v>
       </c>
       <c r="B7" s="164" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -48715,7 +48713,7 @@
         <v>45446</v>
       </c>
       <c r="B8" s="164" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
@@ -48723,7 +48721,7 @@
         <v>45453</v>
       </c>
       <c r="B9" s="164" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
@@ -48731,7 +48729,7 @@
         <v>45474</v>
       </c>
       <c r="B10" s="164" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
@@ -48739,7 +48737,7 @@
         <v>45493</v>
       </c>
       <c r="B11" s="164" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
@@ -48747,7 +48745,7 @@
         <v>45511</v>
       </c>
       <c r="B12" s="164" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
@@ -48755,7 +48753,7 @@
         <v>45523</v>
       </c>
       <c r="B13" s="164" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
@@ -48763,7 +48761,7 @@
         <v>45579</v>
       </c>
       <c r="B14" s="164" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
@@ -48771,7 +48769,7 @@
         <v>45600</v>
       </c>
       <c r="B15" s="164" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
@@ -48779,7 +48777,7 @@
         <v>45607</v>
       </c>
       <c r="B16" s="164" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -48787,7 +48785,7 @@
         <v>45634</v>
       </c>
       <c r="B17" s="164" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
@@ -48795,7 +48793,7 @@
         <v>45651</v>
       </c>
       <c r="B18" s="164" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1"/>
@@ -49807,7 +49805,7 @@
   <sheetData>
     <row r="1" spans="1:97" ht="15.75">
       <c r="A1" s="169" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="164"/>
       <c r="C1" s="164"/>
@@ -49865,7 +49863,7 @@
     </row>
     <row r="3" spans="1:97" ht="32.25" customHeight="1">
       <c r="A3" s="170" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="171">
         <v>45596</v>
@@ -50158,261 +50156,261 @@
     </row>
     <row r="4" spans="1:97" ht="30.75" customHeight="1">
       <c r="A4" s="174" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="175" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="176" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="176" t="s">
+      <c r="D4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="J4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="K4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="L4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="M4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="N4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="O4" s="177" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="E4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="F4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="G4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="H4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="I4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="J4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="K4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="L4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="M4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="N4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="O4" s="177" t="s">
+      <c r="P4" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="R4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="S4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="T4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="U4" s="178" t="s">
         <v>156</v>
       </c>
-      <c r="P4" s="178" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="R4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="S4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="T4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="U4" s="178" t="s">
+      <c r="V4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="W4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="X4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE4" s="203" t="s">
         <v>157</v>
       </c>
-      <c r="V4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="W4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="X4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AB4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AD4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AE4" s="203" t="s">
+      <c r="AF4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AH4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AJ4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL4" s="203" t="s">
         <v>158</v>
       </c>
-      <c r="AF4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AG4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AI4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AJ4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AK4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AL4" s="203" t="s">
+      <c r="AM4" s="177" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN4" s="177" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP4" s="203" t="s">
         <v>159</v>
       </c>
-      <c r="AM4" s="177" t="s">
-        <v>157</v>
-      </c>
-      <c r="AN4" s="177" t="s">
-        <v>157</v>
-      </c>
-      <c r="AO4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP4" s="203" t="s">
+      <c r="AQ4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS4" s="203" t="s">
+        <v>159</v>
+      </c>
+      <c r="AT4" s="179" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AV4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AW4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AX4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AY4" s="203" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BA4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BB4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BC4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BD4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BE4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BF4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BG4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BH4" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="BI4" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="BJ4" s="203" t="s">
+        <v>159</v>
+      </c>
+      <c r="BK4" s="178" t="s">
         <v>160</v>
       </c>
-      <c r="AQ4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AR4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AS4" s="203" t="s">
+      <c r="BL4" s="178" t="s">
         <v>160</v>
       </c>
-      <c r="AT4" s="179" t="s">
-        <v>154</v>
-      </c>
-      <c r="AU4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AV4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AW4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AX4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AY4" s="203" t="s">
+      <c r="BM4" s="178" t="s">
         <v>160</v>
       </c>
-      <c r="AZ4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BB4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BC4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BD4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BE4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BF4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BG4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BH4" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="BI4" s="178" t="s">
-        <v>154</v>
-      </c>
-      <c r="BJ4" s="203" t="s">
+      <c r="BN4" s="178" t="s">
         <v>160</v>
       </c>
-      <c r="BK4" s="178" t="s">
-        <v>161</v>
-      </c>
-      <c r="BL4" s="178" t="s">
-        <v>161</v>
-      </c>
-      <c r="BM4" s="178" t="s">
-        <v>161</v>
-      </c>
-      <c r="BN4" s="178" t="s">
-        <v>161</v>
-      </c>
       <c r="BO4" s="178" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BP4" s="178" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BQ4" s="178" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BR4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BS4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BT4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BX4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BZ4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CA4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CB4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CC4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CD4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CE4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG4" s="177"/>
       <c r="CH4" s="177"/>
       <c r="CI4" s="203" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="CJ4" s="177"/>
       <c r="CK4" s="177"/>
@@ -50424,249 +50422,249 @@
       <c r="CQ4" s="177"/>
       <c r="CR4" s="177"/>
       <c r="CS4" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="174" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P5" s="178" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U5" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE5" s="204"/>
       <c r="AF5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL5" s="204"/>
       <c r="AM5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP5" s="204"/>
       <c r="AQ5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AR5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AS5" s="204"/>
       <c r="AT5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AU5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AV5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AX5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AY5" s="204"/>
       <c r="AZ5" s="177" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BA5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BB5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BC5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BE5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BF5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BG5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BH5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI5" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ5" s="204"/>
       <c r="BK5" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BL5" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BN5" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BO5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BP5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BQ5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BR5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BS5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BT5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BX5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BZ5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CA5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CB5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CC5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CD5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CE5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG5" s="177"/>
       <c r="CH5" s="177"/>
@@ -50681,249 +50679,249 @@
       <c r="CQ5" s="177"/>
       <c r="CR5" s="177"/>
       <c r="CS5" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:97" ht="15.75">
       <c r="A6" s="174" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K6" s="180" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O6" s="177" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P6" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U6" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE6" s="204"/>
       <c r="AF6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL6" s="204"/>
       <c r="AM6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP6" s="204"/>
       <c r="AQ6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS6" s="204"/>
       <c r="AT6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AV6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AY6" s="204"/>
       <c r="AZ6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BA6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BB6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BC6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BE6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BF6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BG6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BH6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI6" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ6" s="204"/>
       <c r="BK6" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BL6" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM6" s="177" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BN6" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BO6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BP6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BQ6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BR6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BS6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BT6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BX6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BZ6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CA6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CB6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CC6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CD6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CE6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG6" s="177"/>
       <c r="CH6" s="177"/>
@@ -50938,198 +50936,198 @@
       <c r="CQ6" s="177"/>
       <c r="CR6" s="177"/>
       <c r="CS6" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="174" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="175" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="J7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="K7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="L7" s="180" t="s">
+        <v>162</v>
+      </c>
+      <c r="M7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="N7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="O7" s="177" t="s">
+        <v>155</v>
+      </c>
+      <c r="P7" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="R7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="S7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="T7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="U7" s="178" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="175" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="G7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="H7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="I7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="J7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="K7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="L7" s="180" t="s">
-        <v>163</v>
-      </c>
-      <c r="M7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="N7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="O7" s="177" t="s">
+      <c r="V7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="W7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="X7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y7" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z7" s="177" t="s">
         <v>156</v>
       </c>
-      <c r="P7" s="178" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="R7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="S7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="T7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="U7" s="178" t="s">
-        <v>166</v>
-      </c>
-      <c r="V7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="W7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="X7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y7" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z7" s="177" t="s">
-        <v>157</v>
-      </c>
       <c r="AA7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE7" s="204"/>
       <c r="AF7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL7" s="204"/>
       <c r="AM7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP7" s="204"/>
       <c r="AQ7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS7" s="204"/>
       <c r="AT7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU7" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AV7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AY7" s="204"/>
       <c r="AZ7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BA7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BB7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BC7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BE7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BF7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BG7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BH7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI7" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ7" s="204"/>
       <c r="BK7" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BL7" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BN7" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BO7" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BP7" s="177"/>
       <c r="BQ7" s="177"/>
@@ -51137,16 +51135,16 @@
       <c r="BS7" s="177"/>
       <c r="BT7" s="177"/>
       <c r="BU7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BX7" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY7" s="177"/>
       <c r="BZ7" s="177"/>
@@ -51172,220 +51170,220 @@
     </row>
     <row r="8" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="174" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="175" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="H8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="J8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="K8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="L8" s="177" t="s">
+        <v>156</v>
+      </c>
+      <c r="M8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="O8" s="177" t="s">
+        <v>155</v>
+      </c>
+      <c r="P8" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="R8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="S8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="T8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="U8" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="V8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="W8" s="177" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="175" t="s">
-        <v>154</v>
-      </c>
-      <c r="C8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="F8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="G8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="H8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="I8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="J8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="K8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="L8" s="177" t="s">
-        <v>157</v>
-      </c>
-      <c r="M8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="N8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="O8" s="177" t="s">
+      <c r="X8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA8" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB8" s="177" t="s">
         <v>156</v>
       </c>
-      <c r="P8" s="178" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="R8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="S8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="T8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="U8" s="178" t="s">
-        <v>154</v>
-      </c>
-      <c r="V8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="W8" s="177" t="s">
-        <v>168</v>
-      </c>
-      <c r="X8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA8" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="AB8" s="177" t="s">
-        <v>157</v>
-      </c>
       <c r="AC8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE8" s="204"/>
       <c r="AF8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL8" s="204"/>
       <c r="AM8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN8" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AO8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP8" s="204"/>
       <c r="AQ8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS8" s="204"/>
       <c r="AT8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AV8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AY8" s="204"/>
       <c r="AZ8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BA8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BB8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BC8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BE8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BF8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BG8" s="177" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BH8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI8" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ8" s="204"/>
       <c r="BK8" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BL8" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BN8" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BO8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BP8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BQ8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BR8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BS8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BT8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW8" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BX8" s="177" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="BY8" s="177"/>
       <c r="BZ8" s="177"/>
@@ -51411,244 +51409,244 @@
     </row>
     <row r="9" spans="1:97" ht="15.75">
       <c r="A9" s="174" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O9" s="180" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P9" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U9" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE9" s="204"/>
       <c r="AF9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL9" s="204"/>
       <c r="AM9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP9" s="204"/>
       <c r="AQ9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS9" s="204"/>
       <c r="AT9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AV9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AY9" s="204"/>
       <c r="AZ9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BA9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BB9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BC9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BE9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BF9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BG9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BH9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI9" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ9" s="204"/>
       <c r="BK9" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BL9" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BN9" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BO9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BP9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BQ9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BR9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BS9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BT9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BX9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BZ9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CA9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CB9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CC9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CD9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CE9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG9" s="177"/>
       <c r="CH9" s="177"/>
@@ -51663,249 +51661,249 @@
       <c r="CQ9" s="177"/>
       <c r="CR9" s="177"/>
       <c r="CS9" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:97" ht="15.75">
       <c r="A10" s="174" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O10" s="177" t="s">
+        <v>155</v>
+      </c>
+      <c r="P10" s="178" t="s">
         <v>156</v>
       </c>
-      <c r="P10" s="178" t="s">
-        <v>157</v>
-      </c>
       <c r="Q10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U10" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE10" s="204"/>
       <c r="AF10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AL10" s="204"/>
       <c r="AM10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AN10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP10" s="204"/>
       <c r="AQ10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS10" s="204"/>
       <c r="AT10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AV10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AY10" s="204"/>
       <c r="AZ10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BA10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BB10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BC10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BD10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BE10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BF10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BG10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BH10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI10" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ10" s="204"/>
       <c r="BK10" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BL10" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BN10" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BO10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BP10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BQ10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BR10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BS10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BT10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW10" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BX10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BZ10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CA10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CB10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CC10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CD10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CE10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG10" s="177"/>
       <c r="CH10" s="177"/>
@@ -51920,249 +51918,249 @@
       <c r="CQ10" s="177"/>
       <c r="CR10" s="177"/>
       <c r="CS10" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:97" ht="15.75">
       <c r="A11" s="174" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="175" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="J11" s="177" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="175" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="D11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="G11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="H11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="I11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="J11" s="177" t="s">
-        <v>174</v>
-      </c>
       <c r="K11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O11" s="177" t="s">
+        <v>155</v>
+      </c>
+      <c r="P11" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="R11" s="177" t="s">
+        <v>153</v>
+      </c>
+      <c r="S11" s="177" t="s">
         <v>156</v>
       </c>
-      <c r="P11" s="178" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="R11" s="177" t="s">
-        <v>154</v>
-      </c>
-      <c r="S11" s="177" t="s">
-        <v>157</v>
-      </c>
       <c r="T11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U11" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE11" s="204"/>
       <c r="AF11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL11" s="204"/>
       <c r="AM11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AN11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP11" s="204"/>
       <c r="AQ11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AR11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AS11" s="204"/>
       <c r="AT11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AV11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AY11" s="204"/>
       <c r="AZ11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BA11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BB11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BC11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BE11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BF11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BG11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BH11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI11" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ11" s="204"/>
       <c r="BK11" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BL11" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BM11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BN11" s="178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BO11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BP11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BQ11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BR11" s="177" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BS11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BT11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BU11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BX11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BZ11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CA11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CB11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CC11" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CD11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CE11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG11" s="177"/>
       <c r="CH11" s="177"/>
@@ -52177,249 +52175,249 @@
       <c r="CQ11" s="177"/>
       <c r="CR11" s="177"/>
       <c r="CS11" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:97" ht="15.75">
       <c r="A12" s="174" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O12" s="177" t="s">
+        <v>155</v>
+      </c>
+      <c r="P12" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q12" s="177" t="s">
         <v>156</v>
       </c>
-      <c r="P12" s="178" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q12" s="177" t="s">
-        <v>157</v>
-      </c>
       <c r="R12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U12" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AB12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AC12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE12" s="204"/>
       <c r="AF12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AI12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AJ12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL12" s="204"/>
       <c r="AM12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AN12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AO12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AP12" s="204"/>
       <c r="AQ12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AR12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AS12" s="204"/>
       <c r="AT12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AU12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AV12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AW12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AY12" s="204"/>
       <c r="AZ12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BA12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BB12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BC12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BD12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BE12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BF12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BG12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BH12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BI12" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BJ12" s="204"/>
       <c r="BK12" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BL12" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BM12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BN12" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BO12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BP12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BQ12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BR12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BS12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BT12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BU12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BV12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BW12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BX12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BY12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BZ12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CA12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CB12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CC12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CD12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CE12" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CG12" s="177"/>
       <c r="CH12" s="177"/>
@@ -52434,249 +52432,249 @@
       <c r="CQ12" s="177"/>
       <c r="CR12" s="177"/>
       <c r="CS12" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:97" ht="15.75">
       <c r="A13" s="174" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" s="175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O13" s="177" t="s">
+        <v>155</v>
+      </c>
+      <c r="P13" s="178" t="s">
         <v>156</v>
       </c>
-      <c r="P13" s="178" t="s">
-        <v>157</v>
-      </c>
       <c r="Q13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U13" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="X13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AB13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AC13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE13" s="205"/>
       <c r="AF13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AI13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AK13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AL13" s="205"/>
       <c r="AM13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AN13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AO13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AP13" s="205"/>
       <c r="AQ13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AR13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AS13" s="205"/>
       <c r="AT13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AU13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AV13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AW13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AX13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AY13" s="205"/>
       <c r="AZ13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BA13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BB13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BC13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BD13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BE13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BF13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BG13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BH13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BI13" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BJ13" s="205"/>
       <c r="BK13" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BL13" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BM13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BN13" s="178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BO13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BP13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BQ13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BR13" s="177" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BS13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BT13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BU13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BV13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BW13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BX13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BY13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BZ13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CA13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CB13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CC13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CD13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CE13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CF13" s="177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CG13" s="177"/>
       <c r="CH13" s="177"/>
@@ -52691,7 +52689,7 @@
       <c r="CQ13" s="177"/>
       <c r="CR13" s="177"/>
       <c r="CS13" s="177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -53713,7 +53711,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="181" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="181" t="s">
         <v>2</v>
@@ -53740,13 +53738,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="185" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="186" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="186" t="s">
+      <c r="L1" s="184" t="s">
         <v>91</v>
-      </c>
-      <c r="L1" s="184" t="s">
-        <v>92</v>
       </c>
       <c r="M1" s="187"/>
       <c r="N1" s="187"/>
@@ -53765,10 +53763,10 @@
     </row>
     <row r="2" spans="1:26" ht="38.25">
       <c r="A2" s="188" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="189" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="190"/>
       <c r="D2" s="190" t="s">
@@ -53795,7 +53793,7 @@
       </c>
       <c r="K2" s="193"/>
       <c r="L2" s="194" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M2" s="187"/>
       <c r="N2" s="187"/>
@@ -53814,13 +53812,13 @@
     </row>
     <row r="3" spans="1:26" ht="51">
       <c r="A3" s="188" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="206" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="195" t="s">
         <v>180</v>
-      </c>
-      <c r="C3" s="195" t="s">
-        <v>181</v>
       </c>
       <c r="D3" s="190" t="s">
         <v>34</v>
@@ -53842,7 +53840,7 @@
       </c>
       <c r="K3" s="191"/>
       <c r="L3" s="194" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M3" s="196"/>
       <c r="N3" s="187"/>
@@ -53861,11 +53859,11 @@
     </row>
     <row r="4" spans="1:26" ht="51">
       <c r="A4" s="188" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="204"/>
       <c r="C4" s="197" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D4" s="190" t="s">
         <v>34</v>
@@ -53887,7 +53885,7 @@
       </c>
       <c r="K4" s="198"/>
       <c r="L4" s="201" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M4" s="196"/>
       <c r="N4" s="187"/>
@@ -53906,13 +53904,13 @@
     </row>
     <row r="5" spans="1:26" ht="51">
       <c r="A5" s="188" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="184" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="190" t="s">
         <v>185</v>
-      </c>
-      <c r="C5" s="190" t="s">
-        <v>186</v>
       </c>
       <c r="D5" s="190" t="s">
         <v>34</v>
@@ -53934,7 +53932,7 @@
       </c>
       <c r="K5" s="191"/>
       <c r="L5" s="194" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M5" s="196"/>
       <c r="N5" s="187"/>

</xml_diff>